<commit_message>
Rcvd Infineon LNA and IF SAW
</commit_message>
<xml_diff>
--- a/bom/front-end-bom.xlsx
+++ b/bom/front-end-bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emastro\Documents\OreSat\GitHub\oresat-c3-rf\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11CD0DD-E261-438A-A0FA-126092713406}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83CA87D-E466-4480-AD38-199ED2175743}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="32220" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3010" yWindow="400" windowWidth="23720" windowHeight="15490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="front-end-eval-boards" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="76">
   <si>
     <t>P</t>
   </si>
@@ -131,15 +131,9 @@
     <t>synthesizer-IF/RF</t>
   </si>
   <si>
-    <t>Last modified: 2019-04-29</t>
-  </si>
-  <si>
     <t>bpf-IF-SAW</t>
   </si>
   <si>
-    <t>EOL</t>
-  </si>
-  <si>
     <t>Qorvo</t>
   </si>
   <si>
@@ -249,6 +243,24 @@
   </si>
   <si>
     <t>bpf-L-band-1</t>
+  </si>
+  <si>
+    <t>JEFF</t>
+  </si>
+  <si>
+    <t>Infineon</t>
+  </si>
+  <si>
+    <t>BGB707L7ESDE6327XTSA1</t>
+  </si>
+  <si>
+    <t>General RF LNA, very low input</t>
+  </si>
+  <si>
+    <t>726-SP000531308</t>
+  </si>
+  <si>
+    <t>Last modified: 2019-07-15</t>
   </si>
 </sst>
 </file>
@@ -268,18 +280,12 @@
       <name val="Sans"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -300,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,9 +329,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -642,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB2B818-5FBF-4232-A5C1-C4802E1712B1}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
@@ -656,7 +659,7 @@
     <col min="4" max="4" width="15.1796875" customWidth="1"/>
     <col min="5" max="5" width="10.6328125" customWidth="1"/>
     <col min="6" max="6" width="15.81640625" customWidth="1"/>
-    <col min="7" max="7" width="22.1796875" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="39" customWidth="1"/>
     <col min="9" max="9" width="13.1796875" customWidth="1"/>
     <col min="10" max="10" width="23.453125" customWidth="1"/>
@@ -703,7 +706,7 @@
     </row>
     <row r="3" spans="1:13" ht="13">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -802,8 +805,8 @@
       <c r="A8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>39</v>
+      <c r="B8" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="C8" s="7">
         <v>10</v>
@@ -835,10 +838,10 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>39</v>
+        <v>48</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="C9" s="7">
         <v>4</v>
@@ -848,19 +851,19 @@
         <v>0</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>2</v>
@@ -870,10 +873,10 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>39</v>
+        <v>49</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="C10" s="7">
         <v>4</v>
@@ -883,19 +886,19 @@
         <v>0</v>
       </c>
       <c r="F10" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="H10" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>2</v>
@@ -905,10 +908,10 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>39</v>
+        <v>50</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="C11" s="7">
         <v>4</v>
@@ -918,19 +921,19 @@
         <v>0</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>2</v>
@@ -940,10 +943,10 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>39</v>
+        <v>51</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="C12" s="7">
         <v>1</v>
@@ -953,16 +956,16 @@
         <v>0</v>
       </c>
       <c r="F12" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="I12" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="7" t="s">
@@ -973,10 +976,10 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>39</v>
+        <v>69</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="C13" s="7">
         <v>3</v>
@@ -986,16 +989,16 @@
         <v>0</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="7" t="s">
@@ -1006,10 +1009,10 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>39</v>
+        <v>59</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="C14" s="7">
         <v>6</v>
@@ -1019,16 +1022,16 @@
         <v>0</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="7" t="s">
@@ -1039,29 +1042,29 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="7" t="s">
@@ -1072,29 +1075,29 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>60</v>
+        <v>65</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="7" t="s">
@@ -1104,67 +1107,89 @@
       <c r="M16" s="8"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="C17" s="7"/>
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="7">
+        <v>4</v>
+      </c>
       <c r="D17" s="8"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="7"/>
+      <c r="E17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="L17" s="7"/>
       <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="C18" s="7"/>
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="7">
+        <v>10</v>
+      </c>
       <c r="D18" s="8"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="7"/>
+      <c r="E18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="L18" s="7"/>
-      <c r="M18" s="8"/>
+      <c r="M18" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="7">
-        <v>10</v>
-      </c>
+      <c r="C19" s="7"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="7"/>
       <c r="L19" s="7"/>
-      <c r="M19" s="8" t="s">
-        <v>70</v>
-      </c>
+      <c r="M19" s="8"/>
     </row>
     <row r="20" spans="1:13">
       <c r="C20" s="7"/>
@@ -1233,55 +1258,42 @@
     </row>
     <row r="25" spans="1:13">
       <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
+      <c r="D25" s="6"/>
       <c r="E25" s="1"/>
       <c r="F25" s="8"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
       <c r="M25" s="8"/>
     </row>
     <row r="26" spans="1:13">
       <c r="C26" s="7"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="1"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
       <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
       <c r="M26" s="8"/>
     </row>
-    <row r="27" spans="1:13">
-      <c r="C27" s="7"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="M27" s="8"/>
-    </row>
-    <row r="28" spans="1:13" ht="13">
-      <c r="A28" s="5" t="s">
+    <row r="27" spans="1:13" ht="13">
+      <c r="A27" s="5" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="29" spans="1:13">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="30" spans="1:13">
-      <c r="A30" t="s">
-        <v>18</v>
+      <c r="A30" s="4">
+        <v>1</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="4">
-        <v>1</v>
-      </c>
-      <c r="B31" s="4" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>